<commit_message>
New omni notebook & fixed interactive explorer
Update of notebooks including fixed interactive explorer and new omni analysis
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{877ABED8-4315-4835-A79E-C05452C3D756}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5760F096-FEDE-4A03-8BFD-C1F83C24E07B}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="30" windowWidth="18075" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="45" windowWidth="28650" windowHeight="20775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trials" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>antenna</t>
   </si>
@@ -161,6 +161,117 @@
   </si>
   <si>
     <t>Hyagi</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Omni</t>
+  </si>
+  <si>
+    <t>centre of omni</t>
+  </si>
+  <si>
+    <t>400 MHz omni, scaled from Cellwave PD620 antenna</t>
+  </si>
+  <si>
+    <t>SAR_file</t>
+  </si>
+  <si>
+    <t>wbSAR-400MHz-monopole.csv</t>
+  </si>
+  <si>
+    <t>omni/400MHz</t>
+  </si>
+  <si>
+    <t>dBiGain</t>
+  </si>
+  <si>
+    <t>horizHPBW</t>
+  </si>
+  <si>
+    <t>vertHPBW</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>omni/70MHz</t>
+  </si>
+  <si>
+    <t>omni/180MHz</t>
+  </si>
+  <si>
+    <t>omni/700MHz</t>
+  </si>
+  <si>
+    <t>omni/1000MHz</t>
+  </si>
+  <si>
+    <t>CELW_PD620_70MHz_monopole.efe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_70MHz_monopole.hfe</t>
+  </si>
+  <si>
+    <t>wbSAR-70MHz-monopole.csv</t>
+  </si>
+  <si>
+    <t>70 MHz omni, scaled from Cellwave PD620 antenna</t>
+  </si>
+  <si>
+    <t>CELW_PD620_180MHz_monopole.efe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_180MHz_monopole.hfe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_400MHz_monopole.efe.zip</t>
+  </si>
+  <si>
+    <t>CELW_PD620_400MHz_monopole.hfe.zip</t>
+  </si>
+  <si>
+    <t>wbSAR-180MHz-monopole.csv</t>
+  </si>
+  <si>
+    <t>CELW_PD620_700MHz_monopole.efe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_700MHz_monopole.hfe</t>
+  </si>
+  <si>
+    <t>wbSAR-700MHz-monopole.csv</t>
+  </si>
+  <si>
+    <t>180 MHz omni, scaled from Cellwave PD620 antenna</t>
+  </si>
+  <si>
+    <t>700 MHz omni, scaled from Cellwave PD620 antenna</t>
+  </si>
+  <si>
+    <t>CELW_PD620_1000MHz_monopole.hfe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_1000MHz_monopole.efe</t>
+  </si>
+  <si>
+    <t>wbSAR-1000MHz-monopole.csv</t>
+  </si>
+  <si>
+    <t>1000 MHz omni, scaled from Cellwave PD620 antenna</t>
   </si>
 </sst>
 </file>
@@ -204,7 +315,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -229,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,14 +378,96 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -342,15 +535,24 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:E20" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A2:E20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:J24" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A2:J24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2"/>
     <tableColumn id="5" xr3:uid="{F0BCB39C-FFB9-4B09-8C46-1A2761995877}" name="3"/>
+    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{41B0189F-E432-43CB-ABF8-5051863B4185}" name="5"/>
+    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,11 +855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,15 +868,20 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -687,11 +894,26 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -707,8 +929,23 @@
       <c r="E3" s="3">
         <v>900</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>70</v>
+      </c>
+      <c r="G3" s="3">
+        <v>180</v>
+      </c>
+      <c r="H3" s="3">
+        <v>400</v>
+      </c>
+      <c r="I3" s="3">
+        <v>700</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -722,8 +959,23 @@
       <c r="E4" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -739,110 +991,195 @@
       <c r="E5" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="3">
+        <v>100</v>
+      </c>
+      <c r="G5" s="3">
+        <v>100</v>
+      </c>
+      <c r="H5" s="3">
+        <v>100</v>
+      </c>
+      <c r="I5" s="3">
+        <v>100</v>
+      </c>
+      <c r="J5" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>7.37</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="I6" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="J6" s="6">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>180</v>
+      </c>
+      <c r="G7" s="3">
+        <v>180</v>
+      </c>
+      <c r="H7" s="3">
+        <v>180</v>
+      </c>
+      <c r="I7" s="3">
+        <v>180</v>
+      </c>
+      <c r="J7" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="10" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="F9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="10">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="10">
-        <v>14</v>
-      </c>
-      <c r="D8" s="10">
-        <v>14</v>
-      </c>
-      <c r="E8" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="10">
-        <v>-7</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="10">
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="E10" s="10">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="10">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D11" s="10">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E11" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="G11" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="H11" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="I11" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="J11" s="6">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -856,44 +1193,89 @@
       <c r="E12" s="10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="10">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="D13" s="10">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="E13" s="10">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D14" s="10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E14" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -907,80 +1289,290 @@
       <c r="E15" s="10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="F15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="10">
+        <v>-3</v>
+      </c>
+      <c r="D16" s="10">
+        <v>-3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>-3</v>
+      </c>
+      <c r="F16" s="10">
+        <v>-12</v>
+      </c>
+      <c r="G16" s="10">
+        <v>-4</v>
+      </c>
+      <c r="H16" s="10">
+        <v>-2.5</v>
+      </c>
+      <c r="I16" s="10">
+        <v>-2.5</v>
+      </c>
+      <c r="J16" s="6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="10">
+        <v>3</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3</v>
+      </c>
+      <c r="E17" s="10">
+        <v>3</v>
+      </c>
+      <c r="F17" s="10">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10">
+        <v>4</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="11" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="F19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="11" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="F20" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="F21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="F22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="7" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
horizontal yagi over ground
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="248" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0825C0C4-E548-4D7A-921D-FB876FC35EF6}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9CA3242-FB32-4DCD-AB52-ABD022CD664E}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="795" windowWidth="28035" windowHeight="20775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="17985" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trials" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
   <si>
     <t>antenna</t>
   </si>
@@ -278,13 +278,31 @@
   </si>
   <si>
     <t>wbSAR-1000MHz-monopole-2022-12-15.csv</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>main beam along y axis</t>
+  </si>
+  <si>
+    <t>2.32GHz horizontal yagi 3m above real ground</t>
+  </si>
+  <si>
+    <t>Hyagi_gnd</t>
+  </si>
+  <si>
+    <t>HYagi_gnd_E_v2.csv</t>
+  </si>
+  <si>
+    <t>HYagi_gnd_H_v2.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +343,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -346,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,11 +414,33 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -543,19 +589,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:J24" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A2:J24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K24" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A2:K24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2"/>
     <tableColumn id="5" xr3:uid="{F0BCB39C-FFB9-4B09-8C46-1A2761995877}" name="3"/>
-    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{41B0189F-E432-43CB-ABF8-5051863B4185}" name="5"/>
-    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -858,11 +905,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G37" sqref="G37"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,14 +924,15 @@
     <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -915,8 +963,11 @@
       <c r="J2" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -947,8 +998,11 @@
       <c r="J3" s="5">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="5">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1031,11 @@
       <c r="J4" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1009,8 +1066,11 @@
       <c r="J5" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -1033,8 +1093,9 @@
       <c r="J6" s="5">
         <v>7.38</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1059,8 +1120,9 @@
       <c r="J7" s="5">
         <v>360</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -1085,8 +1147,9 @@
       <c r="J8" s="5">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1115,8 +1178,11 @@
       <c r="J9" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1147,8 +1213,11 @@
       <c r="J10" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1179,8 +1248,11 @@
       <c r="J11" s="5">
         <v>5.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1211,8 +1283,11 @@
       <c r="J12" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1243,8 +1318,11 @@
       <c r="J13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1275,8 +1353,11 @@
       <c r="J14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1307,8 +1388,11 @@
       <c r="J15" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1339,8 +1423,11 @@
       <c r="J16" s="5">
         <v>-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1371,8 +1458,11 @@
       <c r="J17" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1403,8 +1493,11 @@
       <c r="J18" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1435,8 +1528,11 @@
       <c r="J19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -1465,8 +1561,11 @@
       <c r="J20" s="14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="K20" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1495,8 +1594,11 @@
       <c r="J21" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="K21" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -1525,8 +1627,11 @@
       <c r="J22" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1553,8 +1658,9 @@
       <c r="J23" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -1582,6 +1688,9 @@
       </c>
       <c r="J24" s="5" t="s">
         <v>76</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write up of PD620 omni antenna
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="279" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9CA3242-FB32-4DCD-AB52-ABD022CD664E}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A7CA141-5525-4F4D-8FF8-EC8841D94030}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="17985" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="45" windowWidth="30705" windowHeight="20850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trials" sheetId="2" r:id="rId1"/>
+    <sheet name="trials (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="108">
   <si>
     <t>antenna</t>
   </si>
@@ -296,13 +297,70 @@
   </si>
   <si>
     <t>HYagi_gnd_H_v2.csv</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>omni along z axis</t>
+  </si>
+  <si>
+    <t>omni2/100MHz</t>
+  </si>
+  <si>
+    <t>omni2/1000MHz</t>
+  </si>
+  <si>
+    <t>omni2/3000MHz</t>
+  </si>
+  <si>
+    <t>vertical omni with narrow beam</t>
+  </si>
+  <si>
+    <t>iec62232_omni_1000MHz_100W_0.02m_sampling_NearField.efe.zip</t>
+  </si>
+  <si>
+    <t>iec62232_omni_1000MHz_100W_0.02m_sampling_NearField.hfe.zip</t>
+  </si>
+  <si>
+    <t>iec62232_omni_100MHz_100W_0.1m_sampling_NearField.efe</t>
+  </si>
+  <si>
+    <t>iec62232_omni_100MHz_100W_0.1m_sampling_NearField.hfe</t>
+  </si>
+  <si>
+    <t>wbSAR-100MHz-IEC62232-monopole.csv</t>
+  </si>
+  <si>
+    <t>iec62232_omni_3000MHz_100W_0.02m_sampling_NearField.efe.zip</t>
+  </si>
+  <si>
+    <t>iec62232_omni_3000MHz_100W_0.02m_sampling_NearField.hfe.zip</t>
+  </si>
+  <si>
+    <t>wbSAR-1000MHz-IEC62232-monopole-all.csv</t>
+  </si>
+  <si>
+    <t>wbSAR-3000MHz-IEC62232-monopole-all.csv</t>
+  </si>
+  <si>
+    <t>CELW_PD620_180MHz-SAR-run_monopoleNearField1.efe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_180MHz-SAR-run_monopoleNearField1.hfe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,12 +398,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -414,14 +466,277 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -584,25 +899,47 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K24" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A2:K24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:N24" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A2:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2"/>
     <tableColumn id="5" xr3:uid="{F0BCB39C-FFB9-4B09-8C46-1A2761995877}" name="3"/>
-    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{41B0189F-E432-43CB-ABF8-5051863B4185}" name="5"/>
-    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{034F77D3-3871-4ED6-9BB2-D03FEFB90B4D}" name="10" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{F15FC92D-684F-4252-A179-C9095EDD86B7}" name="11" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{D87AE248-A44F-48FF-B527-01F7C9B6FE7D}" name="12" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C097D44D-2244-43E7-850B-890A6D1E54F1}" name="Table13" displayName="Table13" ref="A2:N24" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A2:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{883C24A5-C1C7-4BED-84DA-F05871C35F01}" name="INPUT" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F0223689-04E2-473D-966B-4E0851A34860}" name="unit" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4932D701-7111-4FCA-AD4F-6B16E96D3D55}" name="1"/>
+    <tableColumn id="4" xr3:uid="{2DA9AC25-7385-4ABB-BB6A-BECFCA80EDF8}" name="2"/>
+    <tableColumn id="5" xr3:uid="{FEEE76E5-5C5B-4616-BC92-C45E3E9773EF}" name="3"/>
+    <tableColumn id="7" xr3:uid="{2E56F92F-24BD-4552-A635-5D1EF47090CE}" name="4" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{08649B7C-EE15-4427-8A17-0A7A589693E2}" name="5"/>
+    <tableColumn id="8" xr3:uid="{20EC8714-10C8-4009-A9F0-5F8E9FC5C771}" name="6" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{9B259623-D14A-4397-92F9-9974E0B8F868}" name="7" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{5314A91F-83B4-47ED-A23F-77E807587C99}" name="8" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{F6D6CA5D-405B-4D7F-B037-A6A07D3A7991}" name="9" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{1D7DAD76-E5CE-4CBA-A8DE-B47F4B611F87}" name="10" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{F5E2A403-0A60-4244-A240-C528B8EDCDF0}" name="11" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{9484C6D6-7504-46BE-89C7-289479FB3CC7}" name="12" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -905,11 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,15 +1261,15 @@
     <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="11" max="14" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -963,11 +1300,20 @@
       <c r="J2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1001,8 +1347,17 @@
       <c r="K3" s="5">
         <v>2320</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="5">
+        <v>100</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N3" s="5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1034,8 +1389,17 @@
       <c r="K4" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1069,8 +1433,17 @@
       <c r="K5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="5">
+        <v>100</v>
+      </c>
+      <c r="M5" s="5">
+        <v>100</v>
+      </c>
+      <c r="N5" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -1094,8 +1467,17 @@
         <v>7.38</v>
       </c>
       <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="M6" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1121,8 +1503,11 @@
         <v>360</v>
       </c>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -1148,8 +1533,11 @@
         <v>20.3</v>
       </c>
       <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1181,8 +1569,17 @@
       <c r="K9" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1216,8 +1613,17 @@
       <c r="K10" s="5">
         <v>-10</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1251,8 +1657,17 @@
       <c r="K11" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="5">
+        <v>20.024999999999999</v>
+      </c>
+      <c r="M11" s="5">
+        <v>10.005000000000001</v>
+      </c>
+      <c r="N11" s="5">
+        <v>10.025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1286,8 +1701,17 @@
       <c r="K12" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1321,8 +1745,17 @@
       <c r="K13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1356,8 +1789,17 @@
       <c r="K14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1391,8 +1833,13 @@
       <c r="K15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1426,8 +1873,17 @@
       <c r="K16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="5">
+        <v>-20</v>
+      </c>
+      <c r="M16" s="5">
+        <v>-4</v>
+      </c>
+      <c r="N16" s="5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1461,8 +1917,17 @@
       <c r="K17" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="5">
+        <v>20</v>
+      </c>
+      <c r="M17" s="5">
+        <v>4</v>
+      </c>
+      <c r="N17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1496,8 +1961,17 @@
       <c r="K18" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1531,8 +2005,17 @@
       <c r="K19" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -1564,8 +2047,17 @@
       <c r="K20" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="L20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1597,8 +2089,17 @@
       <c r="K21" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="L21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -1630,8 +2131,17 @@
       <c r="K22" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1659,8 +2169,17 @@
         <v>82</v>
       </c>
       <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="L23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -1691,6 +2210,43 @@
       </c>
       <c r="K24" s="5" t="s">
         <v>85</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f>(L11-L10)/L12+1</f>
+        <v>201</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ref="M26:N26" si="0">(M11-M10)/M12+1</f>
+        <v>500</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f>(L17-L16)/L18+1</f>
+        <v>401</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:N27" si="1">(M17-M16)/M18+1</f>
+        <v>401</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -1701,4 +2257,1022 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3BE239-38D8-4A92-816A-7F55410339B0}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="14" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>900</v>
+      </c>
+      <c r="D3" s="1">
+        <v>900</v>
+      </c>
+      <c r="E3" s="1">
+        <v>900</v>
+      </c>
+      <c r="F3" s="1">
+        <v>70</v>
+      </c>
+      <c r="G3" s="1">
+        <v>180</v>
+      </c>
+      <c r="H3" s="1">
+        <v>400</v>
+      </c>
+      <c r="I3" s="1">
+        <v>700</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="K3" s="5">
+        <v>2320</v>
+      </c>
+      <c r="L3" s="5">
+        <v>100</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N3" s="5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1">
+        <v>200</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1">
+        <v>100</v>
+      </c>
+      <c r="J5" s="5">
+        <v>100</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>100</v>
+      </c>
+      <c r="M5" s="5">
+        <v>100</v>
+      </c>
+      <c r="N5" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>7.37</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="J6" s="5">
+        <v>7.38</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="M6" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>360</v>
+      </c>
+      <c r="G7" s="1">
+        <v>360</v>
+      </c>
+      <c r="H7" s="1">
+        <v>360</v>
+      </c>
+      <c r="I7" s="1">
+        <v>360</v>
+      </c>
+      <c r="J7" s="5">
+        <v>360</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="5">
+        <v>-10</v>
+      </c>
+      <c r="L10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9">
+        <v>14</v>
+      </c>
+      <c r="D11" s="9">
+        <v>14</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5.05</v>
+      </c>
+      <c r="G11" s="9">
+        <v>5.05</v>
+      </c>
+      <c r="H11" s="9">
+        <v>5.05</v>
+      </c>
+      <c r="I11" s="9">
+        <v>5.05</v>
+      </c>
+      <c r="J11" s="5">
+        <v>5.05</v>
+      </c>
+      <c r="K11" s="5">
+        <v>50</v>
+      </c>
+      <c r="L11" s="5">
+        <v>20.024999999999999</v>
+      </c>
+      <c r="M11" s="5">
+        <v>10.005000000000001</v>
+      </c>
+      <c r="N11" s="5">
+        <v>10.025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-7</v>
+      </c>
+      <c r="D13" s="9">
+        <v>-7</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="9">
+        <v>-3</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-3</v>
+      </c>
+      <c r="E16" s="9">
+        <v>-3</v>
+      </c>
+      <c r="F16" s="9">
+        <v>-12</v>
+      </c>
+      <c r="G16" s="9">
+        <v>-4</v>
+      </c>
+      <c r="H16" s="9">
+        <v>-2.5</v>
+      </c>
+      <c r="I16" s="9">
+        <v>-2.5</v>
+      </c>
+      <c r="J16" s="5">
+        <v>-2</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>-20</v>
+      </c>
+      <c r="M16" s="5">
+        <v>-4</v>
+      </c>
+      <c r="N16" s="5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3</v>
+      </c>
+      <c r="F17" s="9">
+        <v>12</v>
+      </c>
+      <c r="G17" s="9">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="5">
+        <v>2</v>
+      </c>
+      <c r="K17" s="5">
+        <v>2</v>
+      </c>
+      <c r="L17" s="5">
+        <v>20</v>
+      </c>
+      <c r="M17" s="5">
+        <v>4</v>
+      </c>
+      <c r="N17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f>(L11-L10)/L12+1</f>
+        <v>201</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ref="M26:N26" si="0">(M11-M10)/M12+1</f>
+        <v>500</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f>(L17-L16)/L18+1</f>
+        <v>401</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:N27" si="1">(M17-M16)/M18+1</f>
+        <v>401</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update of the PD620 notebook calculations
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="377" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A7CA141-5525-4F4D-8FF8-EC8841D94030}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53B79AF5-1526-4D04-BF71-F239927524DD}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="45" windowWidth="30705" windowHeight="20850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18940" yWindow="830" windowWidth="19200" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trials" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="112">
   <si>
     <t>antenna</t>
   </si>
@@ -354,6 +354,18 @@
   </si>
   <si>
     <t>CELW_PD620_180MHz-SAR-run_monopoleNearField1.hfe</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>CELW_PD620_NearField1.efe</t>
+  </si>
+  <si>
+    <t>CELW_PD620_NearField1.hfe</t>
+  </si>
+  <si>
+    <t>omni/160MHz</t>
   </si>
 </sst>
 </file>
@@ -473,7 +485,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -899,47 +930,52 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:N24" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:N24" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A2:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2"/>
     <tableColumn id="5" xr3:uid="{F0BCB39C-FFB9-4B09-8C46-1A2761995877}" name="3"/>
-    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="19"/>
     <tableColumn id="6" xr3:uid="{41B0189F-E432-43CB-ABF8-5051863B4185}" name="5"/>
-    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{034F77D3-3871-4ED6-9BB2-D03FEFB90B4D}" name="10" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{F15FC92D-684F-4252-A179-C9095EDD86B7}" name="11" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{D87AE248-A44F-48FF-B527-01F7C9B6FE7D}" name="12" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{034F77D3-3871-4ED6-9BB2-D03FEFB90B4D}" name="10" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{F15FC92D-684F-4252-A179-C9095EDD86B7}" name="11" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{D87AE248-A44F-48FF-B527-01F7C9B6FE7D}" name="12" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C097D44D-2244-43E7-850B-890A6D1E54F1}" name="Table13" displayName="Table13" ref="A2:N24" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A2:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{883C24A5-C1C7-4BED-84DA-F05871C35F01}" name="INPUT" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{F0223689-04E2-473D-966B-4E0851A34860}" name="unit" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C097D44D-2244-43E7-850B-890A6D1E54F1}" name="Table13" displayName="Table13" ref="A2:O24" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A2:O24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{883C24A5-C1C7-4BED-84DA-F05871C35F01}" name="INPUT" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{F0223689-04E2-473D-966B-4E0851A34860}" name="unit" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{4932D701-7111-4FCA-AD4F-6B16E96D3D55}" name="1"/>
     <tableColumn id="4" xr3:uid="{2DA9AC25-7385-4ABB-BB6A-BECFCA80EDF8}" name="2"/>
     <tableColumn id="5" xr3:uid="{FEEE76E5-5C5B-4616-BC92-C45E3E9773EF}" name="3"/>
-    <tableColumn id="7" xr3:uid="{2E56F92F-24BD-4552-A635-5D1EF47090CE}" name="4" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2E56F92F-24BD-4552-A635-5D1EF47090CE}" name="4" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{08649B7C-EE15-4427-8A17-0A7A589693E2}" name="5"/>
-    <tableColumn id="8" xr3:uid="{20EC8714-10C8-4009-A9F0-5F8E9FC5C771}" name="6" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{9B259623-D14A-4397-92F9-9974E0B8F868}" name="7" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5314A91F-83B4-47ED-A23F-77E807587C99}" name="8" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{F6D6CA5D-405B-4D7F-B037-A6A07D3A7991}" name="9" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{1D7DAD76-E5CE-4CBA-A8DE-B47F4B611F87}" name="10" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{F5E2A403-0A60-4244-A240-C528B8EDCDF0}" name="11" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{9484C6D6-7504-46BE-89C7-289479FB3CC7}" name="12" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{20EC8714-10C8-4009-A9F0-5F8E9FC5C771}" name="6" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{9B259623-D14A-4397-92F9-9974E0B8F868}" name="7" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{5314A91F-83B4-47ED-A23F-77E807587C99}" name="8" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{F6D6CA5D-405B-4D7F-B037-A6A07D3A7991}" name="9" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{1D7DAD76-E5CE-4CBA-A8DE-B47F4B611F87}" name="10" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{F5E2A403-0A60-4244-A240-C528B8EDCDF0}" name="11" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{9484C6D6-7504-46BE-89C7-289479FB3CC7}" name="12" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{F7AD10B9-F4C8-4C20-94D6-EF033DAFDBF1}" name="13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1249,27 +1285,27 @@
       <selection pane="topRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="14" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" customWidth="1"/>
+    <col min="11" max="14" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1313,7 +1349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1393,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1435,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -1477,7 +1513,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1507,7 +1543,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -1537,7 +1573,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1579,7 +1615,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1623,7 +1659,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1667,7 +1703,7 @@
         <v>10.025</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1747,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1755,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1799,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1839,7 +1875,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1883,7 +1919,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1927,7 +1963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1971,7 +2007,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2051,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -2057,7 +2093,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2099,7 +2135,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -2141,7 +2177,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -2179,7 +2215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -2221,7 +2257,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L26">
         <f>(L11-L10)/L12+1</f>
         <v>201</v>
@@ -2235,7 +2271,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L27">
         <f>(L17-L16)/L18+1</f>
         <v>401</v>
@@ -2261,34 +2297,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3BE239-38D8-4A92-816A-7F55410339B0}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="14" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" customWidth="1"/>
+    <col min="11" max="14" width="21.54296875" customWidth="1"/>
+    <col min="15" max="15" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2331,8 +2368,11 @@
       <c r="N2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2375,8 +2415,11 @@
       <c r="N3" s="5">
         <v>3000</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2417,8 +2460,11 @@
       <c r="N4" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2461,8 +2507,11 @@
       <c r="N5" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -2495,8 +2544,11 @@
       <c r="N6" s="5">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="1">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -2525,8 +2577,11 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -2555,8 +2610,11 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="O8" s="1">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -2597,8 +2655,11 @@
       <c r="N9" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -2641,8 +2702,11 @@
       <c r="N10" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -2685,8 +2749,11 @@
       <c r="N11" s="5">
         <v>10.025</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="9">
+        <v>5.5049999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2729,8 +2796,11 @@
       <c r="N12" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -2773,8 +2843,11 @@
       <c r="N13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -2817,8 +2890,11 @@
       <c r="N14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -2857,8 +2933,11 @@
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -2901,8 +2980,11 @@
       <c r="N16" s="5">
         <v>-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="9">
+        <v>-10.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -2945,8 +3027,11 @@
       <c r="N17" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="9">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -2989,8 +3074,11 @@
       <c r="N18" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -3033,8 +3121,11 @@
       <c r="N19" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -3075,8 +3166,11 @@
       <c r="N20" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="O20" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -3117,8 +3211,11 @@
       <c r="N21" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="O21" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -3159,8 +3256,11 @@
       <c r="N22" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -3197,8 +3297,11 @@
       <c r="N23" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="O23" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -3239,36 +3342,12 @@
       <c r="N24" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L26">
-        <f>(L11-L10)/L12+1</f>
-        <v>201</v>
-      </c>
-      <c r="M26">
-        <f t="shared" ref="M26:N26" si="0">(M11-M10)/M12+1</f>
-        <v>500</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="0"/>
-        <v>501</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L27">
-        <f>(L17-L16)/L18+1</f>
-        <v>401</v>
-      </c>
-      <c r="M27">
-        <f t="shared" ref="M27:N27" si="1">(M17-M16)/M18+1</f>
-        <v>401</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="1"/>
-        <v>401</v>
+      <c r="O24" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
work on point spatial representation
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="396" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53B79AF5-1526-4D04-BF71-F239927524DD}"/>
+  <xr:revisionPtr revIDLastSave="473" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC5D193-90BC-4BCB-BDEB-CF4CA5162955}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="830" windowWidth="19200" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4520" yWindow="1460" windowWidth="28800" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trials" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="119">
   <si>
     <t>antenna</t>
   </si>
@@ -366,6 +366,27 @@
   </si>
   <si>
     <t>omni/160MHz</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>omni2/300MHz</t>
+  </si>
+  <si>
+    <t>iec62232_omni_300MHz_100W_0.02m_sampling_NearField.efe.zip</t>
+  </si>
+  <si>
+    <t>iec62232_omni_300MHz_100W_0.02m_sampling_NearField.hfe.zip</t>
+  </si>
+  <si>
+    <t>wbSAR-300MHz-IEC62232-monopole.csv</t>
+  </si>
+  <si>
+    <t>iec62232_omni_100MHz_100W_0.02m_sampling_NearField.efe.zip</t>
+  </si>
+  <si>
+    <t>iec62232_omni_100MHz_100W_0.02m_sampling_NearField.hfe.zip</t>
   </si>
 </sst>
 </file>
@@ -434,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,11 +502,39 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -874,6 +923,25 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -935,47 +1003,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:N24" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="A2:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:O24" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A2:O24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="INPUT" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit" dataDxfId="22"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="2"/>
     <tableColumn id="5" xr3:uid="{F0BCB39C-FFB9-4B09-8C46-1A2761995877}" name="3"/>
-    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{0E17F9C2-9C3D-40DD-942B-2BB77AD6D080}" name="4" dataDxfId="21"/>
     <tableColumn id="6" xr3:uid="{41B0189F-E432-43CB-ABF8-5051863B4185}" name="5"/>
-    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{034F77D3-3871-4ED6-9BB2-D03FEFB90B4D}" name="10" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{F15FC92D-684F-4252-A179-C9095EDD86B7}" name="11" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{D87AE248-A44F-48FF-B527-01F7C9B6FE7D}" name="12" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{957A7D76-7A12-4C74-BF2B-CBD22383DEB3}" name="6" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{35FE1940-F065-44F6-B3D2-2B148EAAC971}" name="7" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{53C38151-D4E6-4FF4-87F4-340E1CC917C9}" name="8" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{2D674163-5E36-439B-AEA7-594F2A6617D2}" name="9" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{034F77D3-3871-4ED6-9BB2-D03FEFB90B4D}" name="10" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{5E63BB65-4C00-4871-A368-950EB7FE94AF}" name="11" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{F15FC92D-684F-4252-A179-C9095EDD86B7}" name="12" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{D87AE248-A44F-48FF-B527-01F7C9B6FE7D}" name="13" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C097D44D-2244-43E7-850B-890A6D1E54F1}" name="Table13" displayName="Table13" ref="A2:O24" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A2:O24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{883C24A5-C1C7-4BED-84DA-F05871C35F01}" name="INPUT" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{F0223689-04E2-473D-966B-4E0851A34860}" name="unit" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C097D44D-2244-43E7-850B-890A6D1E54F1}" name="Table13" displayName="Table13" ref="A2:P24" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A2:P24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{883C24A5-C1C7-4BED-84DA-F05871C35F01}" name="INPUT" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F0223689-04E2-473D-966B-4E0851A34860}" name="unit" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{4932D701-7111-4FCA-AD4F-6B16E96D3D55}" name="1"/>
     <tableColumn id="4" xr3:uid="{2DA9AC25-7385-4ABB-BB6A-BECFCA80EDF8}" name="2"/>
     <tableColumn id="5" xr3:uid="{FEEE76E5-5C5B-4616-BC92-C45E3E9773EF}" name="3"/>
-    <tableColumn id="7" xr3:uid="{2E56F92F-24BD-4552-A635-5D1EF47090CE}" name="4" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2E56F92F-24BD-4552-A635-5D1EF47090CE}" name="4" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{08649B7C-EE15-4427-8A17-0A7A589693E2}" name="5"/>
-    <tableColumn id="8" xr3:uid="{20EC8714-10C8-4009-A9F0-5F8E9FC5C771}" name="6" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{9B259623-D14A-4397-92F9-9974E0B8F868}" name="7" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{5314A91F-83B4-47ED-A23F-77E807587C99}" name="8" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{F6D6CA5D-405B-4D7F-B037-A6A07D3A7991}" name="9" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{1D7DAD76-E5CE-4CBA-A8DE-B47F4B611F87}" name="10" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{F5E2A403-0A60-4244-A240-C528B8EDCDF0}" name="11" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{9484C6D6-7504-46BE-89C7-289479FB3CC7}" name="12" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{F7AD10B9-F4C8-4C20-94D6-EF033DAFDBF1}" name="13" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{20EC8714-10C8-4009-A9F0-5F8E9FC5C771}" name="6" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{9B259623-D14A-4397-92F9-9974E0B8F868}" name="7" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{5314A91F-83B4-47ED-A23F-77E807587C99}" name="8" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{F6D6CA5D-405B-4D7F-B037-A6A07D3A7991}" name="9" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{1D7DAD76-E5CE-4CBA-A8DE-B47F4B611F87}" name="10" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{8DD32C3A-4876-43B4-A310-FA0338575812}" name="11" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{F5E2A403-0A60-4244-A240-C528B8EDCDF0}" name="12" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{9484C6D6-7504-46BE-89C7-289479FB3CC7}" name="13" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{F7AD10B9-F4C8-4C20-94D6-EF033DAFDBF1}" name="14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1278,11 +1348,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1297,15 +1367,15 @@
     <col min="8" max="8" width="26.453125" customWidth="1"/>
     <col min="9" max="9" width="26.54296875" customWidth="1"/>
     <col min="10" max="10" width="27.1796875" customWidth="1"/>
-    <col min="11" max="14" width="21.54296875" customWidth="1"/>
+    <col min="11" max="15" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1348,8 +1418,11 @@
       <c r="N2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1387,13 +1460,16 @@
         <v>100</v>
       </c>
       <c r="M3" s="5">
+        <v>300</v>
+      </c>
+      <c r="N3" s="5">
         <v>1000</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="5">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1434,8 +1510,11 @@
       <c r="N4" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1478,8 +1557,11 @@
       <c r="N5" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -1512,8 +1594,11 @@
       <c r="N6" s="5">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6" s="5">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1542,8 +1627,9 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -1572,8 +1658,9 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1614,8 +1701,11 @@
       <c r="N9" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O9" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1658,8 +1748,11 @@
       <c r="N10" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O10" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1697,13 +1790,16 @@
         <v>20.024999999999999</v>
       </c>
       <c r="M11" s="5">
+        <v>20.004999999999999</v>
+      </c>
+      <c r="N11" s="5">
         <v>10.005000000000001</v>
       </c>
-      <c r="N11" s="5">
+      <c r="O11" s="5">
         <v>10.025</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1746,8 +1842,11 @@
       <c r="N12" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O12" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1790,8 +1889,11 @@
       <c r="N13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1834,8 +1936,11 @@
       <c r="N14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1872,10 +1977,13 @@
       <c r="L15" s="5">
         <v>0.1</v>
       </c>
-      <c r="M15" s="5"/>
+      <c r="M15" s="5">
+        <v>0.02</v>
+      </c>
       <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1913,13 +2021,16 @@
         <v>-20</v>
       </c>
       <c r="M16" s="5">
-        <v>-4</v>
+        <v>-20</v>
       </c>
       <c r="N16" s="5">
         <v>-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O16" s="5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1957,13 +2068,16 @@
         <v>20</v>
       </c>
       <c r="M17" s="5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="N17" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -2006,8 +2120,11 @@
       <c r="N18" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O18" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -2050,8 +2167,11 @@
       <c r="N19" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O19" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -2087,13 +2207,16 @@
         <v>93</v>
       </c>
       <c r="M20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2126,16 +2249,19 @@
         <v>87</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="M21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -2168,16 +2294,19 @@
         <v>88</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="M22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -2209,13 +2338,16 @@
         <v>101</v>
       </c>
       <c r="M23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -2256,31 +2388,34 @@
       <c r="N24" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L26">
         <f>(L11-L10)/L12+1</f>
         <v>201</v>
       </c>
-      <c r="M26">
-        <f t="shared" ref="M26:N26" si="0">(M11-M10)/M12+1</f>
+      <c r="N26">
+        <f t="shared" ref="N26:O26" si="0">(N11-N10)/N12+1</f>
         <v>500</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <f t="shared" si="0"/>
         <v>501</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L27">
         <f>(L17-L16)/L18+1</f>
         <v>401</v>
       </c>
-      <c r="M27">
-        <f t="shared" ref="M27:N27" si="1">(M17-M16)/M18+1</f>
+      <c r="N27">
+        <f t="shared" ref="N27:O27" si="1">(N17-N16)/N18+1</f>
         <v>401</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <f t="shared" si="1"/>
         <v>401</v>
       </c>
@@ -2297,35 +2432,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3BE239-38D8-4A92-816A-7F55410339B0}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="26.453125" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" customWidth="1"/>
-    <col min="11" max="14" width="21.54296875" customWidth="1"/>
-    <col min="15" max="15" width="22.1796875" customWidth="1"/>
+    <col min="3" max="16" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2371,8 +2497,11 @@
       <c r="O2" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2400,71 +2529,77 @@
       <c r="I3" s="1">
         <v>700</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="2">
         <v>1000</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="2">
         <v>2320</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="2">
         <v>100</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="2">
+        <v>300</v>
+      </c>
+      <c r="N3" s="2">
         <v>1000</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="2">
         <v>3000</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2492,26 +2627,29 @@
       <c r="I5" s="1">
         <v>100</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="2">
         <v>100</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <v>100</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <v>100</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
         <v>100</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -2531,24 +2669,27 @@
       <c r="I6" s="1">
         <v>7.38</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="2">
         <v>7.38</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
         <v>13.5</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <v>13.5</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
         <v>13.5</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="P6" s="1">
         <v>7.38</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -2570,18 +2711,19 @@
       <c r="I7" s="1">
         <v>360</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="2">
         <v>360</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="1">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="1">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -2603,574 +2745,611 @@
       <c r="I8" s="1">
         <v>20.3</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="2">
         <v>20.3</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="1">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="1">
         <v>20.3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="2">
         <v>0.5</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="2">
         <v>-1</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="2">
         <v>-1</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="2">
         <v>0.05</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="2">
         <v>0.05</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="2">
         <v>0.05</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="2">
         <v>0.05</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="2">
         <v>0.05</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="2">
         <v>-10</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P10" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="2">
         <v>14</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="2">
         <v>14</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="2">
         <v>5.05</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="2">
         <v>5.05</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="2">
         <v>5.05</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="2">
         <v>5.05</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="2">
         <v>5.05</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <v>50</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="2">
         <v>20.024999999999999</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="2">
+        <v>20.004999999999999</v>
+      </c>
+      <c r="N11" s="2">
         <v>10.005000000000001</v>
       </c>
-      <c r="N11" s="5">
+      <c r="O11" s="2">
         <v>10.025</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="2">
         <v>5.5049999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="M12" s="5">
+      <c r="C12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="2">
         <v>0.02</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <v>0.02</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="P12" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="2">
         <v>-7</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="2">
         <v>-7</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="2">
         <v>-2</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0</v>
-      </c>
-      <c r="L13" s="5">
-        <v>0</v>
-      </c>
-      <c r="M13" s="5">
-        <v>0</v>
-      </c>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="2">
         <v>7</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="2">
         <v>7</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="9">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <v>0</v>
-      </c>
-      <c r="L14" s="5">
-        <v>0</v>
-      </c>
-      <c r="M14" s="5">
-        <v>0</v>
-      </c>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="2">
         <v>-3</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="2">
         <v>-3</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="2">
         <v>-3</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="2">
         <v>-12</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="2">
         <v>-4</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="2">
         <v>-2.5</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="2">
         <v>-2.5</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="2">
         <v>-2</v>
       </c>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
         <v>-20</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="2">
+        <v>-20</v>
+      </c>
+      <c r="N16" s="2">
         <v>-4</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="2">
         <v>-4</v>
       </c>
-      <c r="O16" s="9">
+      <c r="P16" s="2">
         <v>-10.25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="2">
         <v>3</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="2">
         <v>3</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="2">
         <v>12</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="2">
         <v>4</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="2">
         <v>2.5</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="2">
         <v>2.5</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="2">
         <v>2</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="2">
         <v>2</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="2">
         <v>20</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="2">
+        <v>20</v>
+      </c>
+      <c r="N17" s="2">
         <v>4</v>
       </c>
-      <c r="N17" s="5">
+      <c r="O17" s="2">
         <v>4</v>
       </c>
-      <c r="O17" s="9">
+      <c r="P17" s="2">
         <v>20.25</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="C18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="2">
         <v>0.01</v>
       </c>
-      <c r="L18" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="M18" s="5">
+      <c r="L18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="2">
         <v>0.02</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="2">
         <v>0.02</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="P18" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="O20" s="12" t="s">
+      <c r="P20" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -3206,16 +3385,19 @@
         <v>99</v>
       </c>
       <c r="M21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -3251,16 +3433,19 @@
         <v>100</v>
       </c>
       <c r="M22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="P22" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -3292,16 +3477,19 @@
         <v>101</v>
       </c>
       <c r="M23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="P23" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -3342,7 +3530,10 @@
       <c r="N24" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="O24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="P24" s="6" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plane wave ground calculations
</commit_message>
<xml_diff>
--- a/antennas/spat avg trials.xlsx
+++ b/antennas/spat avg trials.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="473" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC5D193-90BC-4BCB-BDEB-CF4CA5162955}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="11_54798CA6314AABBB858F3E28082CE12B7B06D669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237E4A69-D44F-4F09-962D-814EC92B356C}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="1460" windowWidth="28800" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1351,8 +1351,8 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L22" sqref="L22"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1834,7 +1834,7 @@
         <v>0.1</v>
       </c>
       <c r="L12" s="5">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M12" s="5">
         <v>0.02</v>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M15" s="5">
         <v>0.02</v>
@@ -2112,7 +2112,7 @@
         <v>0.01</v>
       </c>
       <c r="L18" s="5">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M18" s="5">
         <v>0.02</v>
@@ -2395,7 +2395,7 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L26">
         <f>(L11-L10)/L12+1</f>
-        <v>201</v>
+        <v>1001</v>
       </c>
       <c r="N26">
         <f t="shared" ref="N26:O26" si="0">(N11-N10)/N12+1</f>
@@ -2409,7 +2409,7 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L27">
         <f>(L17-L16)/L18+1</f>
-        <v>401</v>
+        <v>2001</v>
       </c>
       <c r="N27">
         <f t="shared" ref="N27:O27" si="1">(N17-N16)/N18+1</f>

</xml_diff>